<commit_message>
swapped organ and body part in samples sheet as it was wrong way round
</commit_message>
<xml_diff>
--- a/2017-10/SmartSeq2/Q3DemoSS2Metadata.xlsx
+++ b/2017-10/SmartSeq2/Q3DemoSS2Metadata.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28702"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbergin/Documents/HCA/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jupp/dev/hca/demo-data/2017-10/SmartSeq2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="780" yWindow="460" windowWidth="25600" windowHeight="13860" activeTab="6"/>
+    <workbookView xWindow="780" yWindow="460" windowWidth="25600" windowHeight="13860" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="project" sheetId="1" r:id="rId1"/>
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -716,7 +716,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
@@ -811,7 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
reverted back to keep sample as it was organ=glioblastoma
</commit_message>
<xml_diff>
--- a/2017-10/SmartSeq2/Q3DemoSS2Metadata.xlsx
+++ b/2017-10/SmartSeq2/Q3DemoSS2Metadata.xlsx
@@ -677,7 +677,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,7 +707,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -716,7 +716,7 @@
         <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>

</xml_diff>